<commit_message>
JSExecutor Use cases Incorporated
</commit_message>
<xml_diff>
--- a/src/test/resources/user_files/filters.xlsx
+++ b/src/test/resources/user_files/filters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPAM\ATMP\Workspace\ATMP-Advanced\src\test\resources\user_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CF7501-8C01-4218-BA9B-26516CB4BE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77058CF6-599B-4958-A7D0-F6FC66FA9B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="US1-Create" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>FilterName</t>
   </si>
@@ -170,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -186,6 +186,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -588,10 +591,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E0C955E-3317-4651-BA49-DD05F4264714}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,6 +617,16 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -623,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7591E56-44AB-4A48-8B56-43D7DFC40262}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>